<commit_message>
Update on translations to L
</commit_message>
<xml_diff>
--- a/snomed/volven-8352-snomed.xlsx
+++ b/snomed/volven-8352-snomed.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Anatomisk lokalisasjon" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Anatomisk lokalisasjon'!$A$1:$M$311</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Anatomisk lokalisasjon'!$A$1:$M$312</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="742">
   <si>
     <t>Kode</t>
   </si>
@@ -2150,13 +2150,115 @@
   </si>
   <si>
     <t>69536005 | Head structure (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61563008 | Epiglottis structure (body structure) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">87644002 | Epididymis structure (body structure) </t>
+  </si>
+  <si>
+    <t>Prosedyre?</t>
+  </si>
+  <si>
+    <t>367601008 | Fauces structure (body structure)</t>
+  </si>
+  <si>
+    <t>362806007 | Dorsum of foot (surface region) (body structure)</t>
+  </si>
+  <si>
+    <t>Må velge mellom store og lille</t>
+  </si>
+  <si>
+    <t>66106009 | Structure of lesser supraclavicular fossa (body structure)</t>
+  </si>
+  <si>
+    <t>79087004 | Structure of greater supraclavicular fossa (body structure)</t>
+  </si>
+  <si>
+    <t>FSU-2</t>
+  </si>
+  <si>
+    <t>Furunkel: Smertefull, rød nodulus som gradvis omdannes til en større pustel med sentral nekrose. Hyppigst lokalisert til ansikt, hals, armer, fingre og nates.</t>
+  </si>
+  <si>
+    <t>72914001 | Palatal structure (body structure)</t>
+  </si>
+  <si>
+    <t>28231008 | Gallbladder structure (body structure)</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>87176006 | Bartholin's gland structure (body structure)</t>
+  </si>
+  <si>
+    <t>182349006 | Genital region (body structure)</t>
+  </si>
+  <si>
+    <t>Struktur, område eller system?</t>
+  </si>
+  <si>
+    <t>28273000 | Bile duct structure (body structure)</t>
+  </si>
+  <si>
+    <t>113279002 | Gingival structure (body structure)</t>
+  </si>
+  <si>
+    <t>60319009 | Glans penis structure (body structure)</t>
+  </si>
+  <si>
+    <t>46862004 | Buttock structure (body structure)</t>
+  </si>
+  <si>
+    <t>45289007 | Parotid gland structure (body structure)</t>
+  </si>
+  <si>
+    <t>88481005 | Sublingual gland structure (body structure) </t>
+  </si>
+  <si>
+    <t>181235001 | Entire submandibular gland (body structure</t>
+  </si>
+  <si>
+    <t>69748006 | Thyroid structure (body structure)</t>
+  </si>
+  <si>
+    <t>30291003 | Chin structure (body structure)</t>
+  </si>
+  <si>
+    <t>49928004 | Structure of anterior portion of neck (body structure)</t>
+  </si>
+  <si>
+    <t>73897004 | Skin structure of face (body structure)</t>
+  </si>
+  <si>
+    <t>76261009 | Skin structure of axilla (body structure)</t>
+  </si>
+  <si>
+    <t>63125000 | Structure of dorsum of hand (body structure) </t>
+  </si>
+  <si>
+    <t>102297006 | Main bronchus structure (body structure)</t>
+  </si>
+  <si>
+    <t>64688005 | Bone structure of coccyx (body structure) </t>
+  </si>
+  <si>
+    <t>76853006 | Heel structure (body structure) </t>
+  </si>
+  <si>
+    <t>21547004 | Palm (region) structure (body structure) </t>
+  </si>
+  <si>
+    <t>1231004 | Meninges structure (body structure)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2290,6 +2392,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2633,7 +2741,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -2641,6 +2749,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2718,6 +2829,7 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2835,11 +2947,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="200798856"/>
-        <c:axId val="200800032"/>
+        <c:axId val="199693360"/>
+        <c:axId val="199696104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200798856"/>
+        <c:axId val="199693360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2882,7 +2994,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200800032"/>
+        <c:crossAx val="199696104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2890,7 +3002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200800032"/>
+        <c:axId val="199696104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2941,7 +3053,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200798856"/>
+        <c:crossAx val="199693360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2955,6 +3067,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3613,7 +3726,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Bjørn Næss" refreshedDate="42626.614281249997" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="310">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:M311" sheet="Anatomisk lokalisasjon"/>
+    <worksheetSource ref="A1:M312" sheet="Anatomisk lokalisasjon"/>
   </cacheSource>
   <cacheFields count="13">
     <cacheField name="Kodeverk" numFmtId="0">
@@ -8421,7 +8534,7 @@
   <dimension ref="A3:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8471,10 +8584,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M311"/>
+  <dimension ref="A1:M312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8528,7 +8641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>620</v>
       </c>
@@ -8579,7 +8692,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>620</v>
       </c>
@@ -8603,7 +8716,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8624,7 +8737,7 @@
         <v>42626</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>620</v>
       </c>
@@ -8648,7 +8761,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>620</v>
       </c>
@@ -8696,7 +8809,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>620</v>
       </c>
@@ -8720,7 +8833,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>620</v>
       </c>
@@ -8744,7 +8857,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>620</v>
       </c>
@@ -8785,14 +8898,14 @@
       <c r="E12" t="s">
         <v>643</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" t="s">
+        <v>672</v>
       </c>
       <c r="J12" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>620</v>
       </c>
@@ -8816,7 +8929,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>620</v>
       </c>
@@ -8840,7 +8953,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>620</v>
       </c>
@@ -8885,7 +8998,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>620</v>
       </c>
@@ -8957,7 +9070,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>620</v>
       </c>
@@ -8981,7 +9094,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>620</v>
       </c>
@@ -9005,7 +9118,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>620</v>
       </c>
@@ -9043,14 +9156,14 @@
       <c r="D23" t="s">
         <v>48</v>
       </c>
-      <c r="F23">
-        <v>-1</v>
+      <c r="F23" t="s">
+        <v>677</v>
       </c>
       <c r="J23" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>620</v>
       </c>
@@ -9077,7 +9190,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>620</v>
       </c>
@@ -9115,14 +9228,14 @@
       <c r="D26" t="s">
         <v>54</v>
       </c>
-      <c r="F26">
-        <v>-1</v>
+      <c r="F26" t="s">
+        <v>677</v>
       </c>
       <c r="J26" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>620</v>
       </c>
@@ -9203,7 +9316,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>620</v>
       </c>
@@ -9227,7 +9340,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>620</v>
       </c>
@@ -9251,7 +9364,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>620</v>
       </c>
@@ -9275,7 +9388,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>620</v>
       </c>
@@ -9299,7 +9412,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>620</v>
       </c>
@@ -9326,7 +9439,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>620</v>
       </c>
@@ -9374,7 +9487,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>620</v>
       </c>
@@ -9398,7 +9511,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>620</v>
       </c>
@@ -9467,7 +9580,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>620</v>
       </c>
@@ -9539,7 +9652,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>620</v>
       </c>
@@ -9587,7 +9700,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>620</v>
       </c>
@@ -9649,8 +9762,8 @@
       <c r="D48" t="s">
         <v>99</v>
       </c>
-      <c r="F48">
-        <v>-1</v>
+      <c r="F48" t="s">
+        <v>677</v>
       </c>
       <c r="J48" s="1">
         <v>41752</v>
@@ -9743,7 +9856,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>620</v>
       </c>
@@ -9815,7 +9928,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>620</v>
       </c>
@@ -9842,7 +9955,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>620</v>
       </c>
@@ -9856,14 +9969,14 @@
       <c r="D57" t="s">
         <v>116</v>
       </c>
-      <c r="F57">
-        <v>-1</v>
+      <c r="F57" t="s">
+        <v>677</v>
       </c>
       <c r="J57" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>620</v>
       </c>
@@ -9901,6 +10014,12 @@
       <c r="D59" t="s">
         <v>120</v>
       </c>
+      <c r="E59" t="s">
+        <v>708</v>
+      </c>
+      <c r="F59" t="s">
+        <v>653</v>
+      </c>
       <c r="J59" s="1">
         <v>41752</v>
       </c>
@@ -9919,6 +10038,12 @@
       <c r="D60" t="s">
         <v>122</v>
       </c>
+      <c r="E60" t="s">
+        <v>709</v>
+      </c>
+      <c r="F60" t="s">
+        <v>653</v>
+      </c>
       <c r="J60" s="1">
         <v>41752</v>
       </c>
@@ -9937,11 +10062,17 @@
       <c r="D61" t="s">
         <v>124</v>
       </c>
+      <c r="F61" t="s">
+        <v>634</v>
+      </c>
+      <c r="H61" t="s">
+        <v>710</v>
+      </c>
       <c r="J61" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>620</v>
       </c>
@@ -9976,11 +10107,17 @@
       <c r="D63" t="s">
         <v>128</v>
       </c>
+      <c r="E63" t="s">
+        <v>711</v>
+      </c>
+      <c r="F63" t="s">
+        <v>653</v>
+      </c>
       <c r="J63" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>620</v>
       </c>
@@ -9997,8 +10134,8 @@
       <c r="E64" t="s">
         <v>689</v>
       </c>
-      <c r="F64">
-        <v>-1</v>
+      <c r="F64" t="s">
+        <v>672</v>
       </c>
       <c r="H64" t="s">
         <v>690</v>
@@ -10007,7 +10144,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>620</v>
       </c>
@@ -10021,8 +10158,8 @@
       <c r="D65" t="s">
         <v>132</v>
       </c>
-      <c r="F65">
-        <v>-1</v>
+      <c r="F65" t="s">
+        <v>677</v>
       </c>
       <c r="J65" s="1">
         <v>41752</v>
@@ -10057,7 +10194,7 @@
         <v>620</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B130" si="1">LEFT(C67,1)</f>
+        <f t="shared" ref="B67:B131" si="1">LEFT(C67,1)</f>
         <v>F</v>
       </c>
       <c r="C67" t="s">
@@ -10172,7 +10309,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>620</v>
       </c>
@@ -10220,7 +10357,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>620</v>
       </c>
@@ -10234,14 +10371,14 @@
       <c r="D74" t="s">
         <v>150</v>
       </c>
-      <c r="F74">
-        <v>-1</v>
+      <c r="F74" t="s">
+        <v>677</v>
       </c>
       <c r="J74" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>620</v>
       </c>
@@ -10255,8 +10392,8 @@
       <c r="D75" t="s">
         <v>130</v>
       </c>
-      <c r="F75">
-        <v>-1</v>
+      <c r="F75" t="s">
+        <v>677</v>
       </c>
       <c r="I75" s="1">
         <v>42614</v>
@@ -10268,7 +10405,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>620</v>
       </c>
@@ -10316,7 +10453,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>620</v>
       </c>
@@ -10330,14 +10467,14 @@
       <c r="D78" t="s">
         <v>157</v>
       </c>
-      <c r="F78">
-        <v>-1</v>
+      <c r="F78" t="s">
+        <v>677</v>
       </c>
       <c r="J78" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>620</v>
       </c>
@@ -10351,14 +10488,14 @@
       <c r="D79" t="s">
         <v>159</v>
       </c>
-      <c r="F79">
-        <v>-1</v>
+      <c r="F79" t="s">
+        <v>677</v>
       </c>
       <c r="J79" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>620</v>
       </c>
@@ -10372,8 +10509,8 @@
       <c r="D80" t="s">
         <v>161</v>
       </c>
-      <c r="F80">
-        <v>-1</v>
+      <c r="F80" t="s">
+        <v>677</v>
       </c>
       <c r="J80" s="1">
         <v>41752</v>
@@ -10403,7 +10540,7 @@
         <v>41752</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>620</v>
       </c>
@@ -10417,8 +10554,8 @@
       <c r="D82" t="s">
         <v>165</v>
       </c>
-      <c r="F82">
-        <v>-1</v>
+      <c r="F82" t="s">
+        <v>677</v>
       </c>
       <c r="J82" s="1">
         <v>41752</v>
@@ -10438,11 +10575,17 @@
       <c r="D83" t="s">
         <v>167</v>
       </c>
+      <c r="E83" t="s">
+        <v>712</v>
+      </c>
+      <c r="F83" t="s">
+        <v>653</v>
+      </c>
       <c r="J83" s="1">
         <v>41752</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>620</v>
       </c>
@@ -10477,6 +10620,15 @@
       <c r="D85" t="s">
         <v>171</v>
       </c>
+      <c r="E85" t="s">
+        <v>714</v>
+      </c>
+      <c r="F85" t="s">
+        <v>677</v>
+      </c>
+      <c r="H85" t="s">
+        <v>713</v>
+      </c>
       <c r="J85" s="1">
         <v>41752</v>
       </c>
@@ -10490,14 +10642,18 @@
         <v>F</v>
       </c>
       <c r="C86" t="s">
-        <v>172</v>
+        <v>716</v>
       </c>
       <c r="D86" t="s">
-        <v>173</v>
-      </c>
-      <c r="J86" s="1">
-        <v>41752</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E86" t="s">
+        <v>715</v>
+      </c>
+      <c r="F86" t="s">
+        <v>677</v>
+      </c>
+      <c r="J86" s="1"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
@@ -10505,13 +10661,19 @@
       </c>
       <c r="B87" t="str">
         <f t="shared" si="1"/>
-        <v>G</v>
+        <v>F</v>
       </c>
       <c r="C87" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D87" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="F87" t="s">
+        <v>634</v>
+      </c>
+      <c r="H87" t="s">
+        <v>717</v>
       </c>
       <c r="J87" s="1">
         <v>41752</v>
@@ -10526,10 +10688,16 @@
         <v>G</v>
       </c>
       <c r="C88" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D88" t="s">
-        <v>177</v>
+        <v>175</v>
+      </c>
+      <c r="E88" t="s">
+        <v>718</v>
+      </c>
+      <c r="F88" t="s">
+        <v>653</v>
       </c>
       <c r="J88" s="1">
         <v>41752</v>
@@ -10544,10 +10712,16 @@
         <v>G</v>
       </c>
       <c r="C89" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D89" t="s">
-        <v>179</v>
+        <v>177</v>
+      </c>
+      <c r="F89" t="s">
+        <v>634</v>
+      </c>
+      <c r="H89" t="s">
+        <v>710</v>
       </c>
       <c r="J89" s="1">
         <v>41752</v>
@@ -10562,10 +10736,16 @@
         <v>G</v>
       </c>
       <c r="C90" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D90" t="s">
-        <v>181</v>
+        <v>179</v>
+      </c>
+      <c r="E90" t="s">
+        <v>719</v>
+      </c>
+      <c r="F90" t="s">
+        <v>653</v>
       </c>
       <c r="J90" s="1">
         <v>41752</v>
@@ -10580,10 +10760,16 @@
         <v>G</v>
       </c>
       <c r="C91" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D91" t="s">
-        <v>183</v>
+        <v>181</v>
+      </c>
+      <c r="E91" t="s">
+        <v>721</v>
+      </c>
+      <c r="F91" t="s">
+        <v>653</v>
       </c>
       <c r="J91" s="1">
         <v>41752</v>
@@ -10598,10 +10784,19 @@
         <v>G</v>
       </c>
       <c r="C92" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D92" t="s">
-        <v>185</v>
+        <v>183</v>
+      </c>
+      <c r="E92" t="s">
+        <v>722</v>
+      </c>
+      <c r="F92" t="s">
+        <v>672</v>
+      </c>
+      <c r="H92" t="s">
+        <v>723</v>
       </c>
       <c r="J92" s="1">
         <v>41752</v>
@@ -10616,10 +10811,16 @@
         <v>G</v>
       </c>
       <c r="C93" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D93" t="s">
-        <v>187</v>
+        <v>185</v>
+      </c>
+      <c r="E93" t="s">
+        <v>724</v>
+      </c>
+      <c r="F93" t="s">
+        <v>672</v>
       </c>
       <c r="J93" s="1">
         <v>41752</v>
@@ -10634,10 +10835,16 @@
         <v>G</v>
       </c>
       <c r="C94" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D94" t="s">
-        <v>189</v>
+        <v>187</v>
+      </c>
+      <c r="E94" t="s">
+        <v>725</v>
+      </c>
+      <c r="F94" t="s">
+        <v>653</v>
       </c>
       <c r="J94" s="1">
         <v>41752</v>
@@ -10652,10 +10859,16 @@
         <v>G</v>
       </c>
       <c r="C95" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D95" t="s">
-        <v>191</v>
+        <v>189</v>
+      </c>
+      <c r="E95" t="s">
+        <v>726</v>
+      </c>
+      <c r="F95" t="s">
+        <v>653</v>
       </c>
       <c r="J95" s="1">
         <v>41752</v>
@@ -10670,10 +10883,16 @@
         <v>G</v>
       </c>
       <c r="C96" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D96" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="E96" t="s">
+        <v>727</v>
+      </c>
+      <c r="F96" t="s">
+        <v>653</v>
       </c>
       <c r="J96" s="1">
         <v>41752</v>
@@ -10688,10 +10907,16 @@
         <v>G</v>
       </c>
       <c r="C97" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D97" t="s">
-        <v>195</v>
+        <v>193</v>
+      </c>
+      <c r="E97" t="s">
+        <v>728</v>
+      </c>
+      <c r="F97" t="s">
+        <v>672</v>
       </c>
       <c r="J97" s="1">
         <v>41752</v>
@@ -10706,10 +10931,16 @@
         <v>G</v>
       </c>
       <c r="C98" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D98" t="s">
-        <v>197</v>
+        <v>195</v>
+      </c>
+      <c r="E98" t="s">
+        <v>729</v>
+      </c>
+      <c r="F98" t="s">
+        <v>653</v>
       </c>
       <c r="J98" s="1">
         <v>41752</v>
@@ -10724,10 +10955,16 @@
         <v>G</v>
       </c>
       <c r="C99" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D99" t="s">
-        <v>199</v>
+        <v>197</v>
+      </c>
+      <c r="E99" t="s">
+        <v>730</v>
+      </c>
+      <c r="F99" t="s">
+        <v>653</v>
       </c>
       <c r="J99" s="1">
         <v>41752</v>
@@ -10739,13 +10976,19 @@
       </c>
       <c r="B100" t="str">
         <f t="shared" si="1"/>
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="C100" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D100" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="E100" t="s">
+        <v>731</v>
+      </c>
+      <c r="F100" t="s">
+        <v>653</v>
       </c>
       <c r="J100" s="1">
         <v>41752</v>
@@ -10760,10 +11003,16 @@
         <v>H</v>
       </c>
       <c r="C101" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D101" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E101" t="s">
+        <v>732</v>
+      </c>
+      <c r="F101" t="s">
+        <v>653</v>
       </c>
       <c r="J101" s="1">
         <v>41752</v>
@@ -10778,10 +11027,16 @@
         <v>H</v>
       </c>
       <c r="C102" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D102" t="s">
-        <v>205</v>
+        <v>203</v>
+      </c>
+      <c r="E102" t="s">
+        <v>733</v>
+      </c>
+      <c r="F102" t="s">
+        <v>653</v>
       </c>
       <c r="J102" s="1">
         <v>41752</v>
@@ -10796,10 +11051,16 @@
         <v>H</v>
       </c>
       <c r="C103" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D103" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="E103" t="s">
+        <v>734</v>
+      </c>
+      <c r="F103" t="s">
+        <v>653</v>
       </c>
       <c r="J103" s="1">
         <v>41752</v>
@@ -10814,10 +11075,16 @@
         <v>H</v>
       </c>
       <c r="C104" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D104" t="s">
-        <v>209</v>
+        <v>207</v>
+      </c>
+      <c r="E104" t="s">
+        <v>735</v>
+      </c>
+      <c r="F104" t="s">
+        <v>653</v>
       </c>
       <c r="J104" s="1">
         <v>41752</v>
@@ -10832,10 +11099,16 @@
         <v>H</v>
       </c>
       <c r="C105" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D105" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="E105" t="s">
+        <v>736</v>
+      </c>
+      <c r="F105" t="s">
+        <v>653</v>
       </c>
       <c r="J105" s="1">
         <v>41752</v>
@@ -10850,10 +11123,16 @@
         <v>H</v>
       </c>
       <c r="C106" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D106" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="E106" t="s">
+        <v>737</v>
+      </c>
+      <c r="F106" t="s">
+        <v>653</v>
       </c>
       <c r="J106" s="1">
         <v>41752</v>
@@ -10868,10 +11147,16 @@
         <v>H</v>
       </c>
       <c r="C107" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D107" t="s">
-        <v>215</v>
+        <v>213</v>
+      </c>
+      <c r="E107" t="s">
+        <v>738</v>
+      </c>
+      <c r="F107" t="s">
+        <v>720</v>
       </c>
       <c r="J107" s="1">
         <v>41752</v>
@@ -10886,10 +11171,16 @@
         <v>H</v>
       </c>
       <c r="C108" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D108" t="s">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="E108" t="s">
+        <v>739</v>
+      </c>
+      <c r="F108" t="s">
+        <v>653</v>
       </c>
       <c r="J108" s="1">
         <v>41752</v>
@@ -10904,13 +11195,13 @@
         <v>H</v>
       </c>
       <c r="C109" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D109" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E109" t="s">
-        <v>704</v>
+        <v>740</v>
       </c>
       <c r="F109" t="s">
         <v>653</v>
@@ -10928,13 +11219,13 @@
         <v>H</v>
       </c>
       <c r="C110" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D110" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E110" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F110" t="s">
         <v>653</v>
@@ -10952,10 +11243,16 @@
         <v>H</v>
       </c>
       <c r="C111" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D111" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="E111" t="s">
+        <v>705</v>
+      </c>
+      <c r="F111" t="s">
+        <v>653</v>
       </c>
       <c r="J111" s="1">
         <v>41752</v>
@@ -10970,10 +11267,16 @@
         <v>H</v>
       </c>
       <c r="C112" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D112" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="E112" t="s">
+        <v>741</v>
+      </c>
+      <c r="F112" t="s">
+        <v>720</v>
       </c>
       <c r="J112" s="1">
         <v>41752</v>
@@ -10988,10 +11291,13 @@
         <v>H</v>
       </c>
       <c r="C113" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D113" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>741</v>
       </c>
       <c r="J113" s="1">
         <v>41752</v>
@@ -11006,16 +11312,10 @@
         <v>H</v>
       </c>
       <c r="C114" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D114" t="s">
-        <v>229</v>
-      </c>
-      <c r="E114" t="s">
-        <v>706</v>
-      </c>
-      <c r="F114" t="s">
-        <v>653</v>
+        <v>227</v>
       </c>
       <c r="J114" s="1">
         <v>41752</v>
@@ -11030,10 +11330,16 @@
         <v>H</v>
       </c>
       <c r="C115" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D115" t="s">
-        <v>231</v>
+        <v>229</v>
+      </c>
+      <c r="E115" t="s">
+        <v>706</v>
+      </c>
+      <c r="F115" t="s">
+        <v>653</v>
       </c>
       <c r="J115" s="1">
         <v>41752</v>
@@ -11048,16 +11354,10 @@
         <v>H</v>
       </c>
       <c r="C116" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D116" t="s">
-        <v>233</v>
-      </c>
-      <c r="E116" t="s">
-        <v>707</v>
-      </c>
-      <c r="F116" t="s">
-        <v>653</v>
+        <v>231</v>
       </c>
       <c r="J116" s="1">
         <v>41752</v>
@@ -11072,10 +11372,16 @@
         <v>H</v>
       </c>
       <c r="C117" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D117" t="s">
-        <v>235</v>
+        <v>233</v>
+      </c>
+      <c r="E117" t="s">
+        <v>707</v>
+      </c>
+      <c r="F117" t="s">
+        <v>653</v>
       </c>
       <c r="J117" s="1">
         <v>41752</v>
@@ -11090,10 +11396,10 @@
         <v>H</v>
       </c>
       <c r="C118" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D118" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J118" s="1">
         <v>41752</v>
@@ -11108,10 +11414,10 @@
         <v>H</v>
       </c>
       <c r="C119" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D119" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J119" s="1">
         <v>41752</v>
@@ -11126,10 +11432,10 @@
         <v>H</v>
       </c>
       <c r="C120" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D120" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J120" s="1">
         <v>41752</v>
@@ -11144,10 +11450,10 @@
         <v>H</v>
       </c>
       <c r="C121" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D121" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J121" s="1">
         <v>41752</v>
@@ -11159,13 +11465,13 @@
       </c>
       <c r="B122" t="str">
         <f t="shared" si="1"/>
-        <v>I</v>
+        <v>H</v>
       </c>
       <c r="C122" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D122" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J122" s="1">
         <v>41752</v>
@@ -11180,10 +11486,10 @@
         <v>I</v>
       </c>
       <c r="C123" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D123" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J123" s="1">
         <v>41752</v>
@@ -11198,10 +11504,10 @@
         <v>I</v>
       </c>
       <c r="C124" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D124" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J124" s="1">
         <v>41752</v>
@@ -11216,10 +11522,10 @@
         <v>I</v>
       </c>
       <c r="C125" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D125" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J125" s="1">
         <v>41752</v>
@@ -11234,10 +11540,10 @@
         <v>I</v>
       </c>
       <c r="C126" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D126" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J126" s="1">
         <v>41752</v>
@@ -11249,13 +11555,13 @@
       </c>
       <c r="B127" t="str">
         <f t="shared" si="1"/>
-        <v>J</v>
+        <v>I</v>
       </c>
       <c r="C127" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D127" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J127" s="1">
         <v>41752</v>
@@ -11267,13 +11573,13 @@
       </c>
       <c r="B128" t="str">
         <f t="shared" si="1"/>
-        <v>K</v>
+        <v>J</v>
       </c>
       <c r="C128" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D128" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J128" s="1">
         <v>41752</v>
@@ -11288,10 +11594,10 @@
         <v>K</v>
       </c>
       <c r="C129" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D129" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J129" s="1">
         <v>41752</v>
@@ -11306,10 +11612,10 @@
         <v>K</v>
       </c>
       <c r="C130" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D130" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J130" s="1">
         <v>41752</v>
@@ -11320,14 +11626,14 @@
         <v>620</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" ref="B131:B194" si="2">LEFT(C131,1)</f>
+        <f t="shared" si="1"/>
         <v>K</v>
       </c>
       <c r="C131" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D131" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J131" s="1">
         <v>41752</v>
@@ -11338,14 +11644,14 @@
         <v>620</v>
       </c>
       <c r="B132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B132:B195" si="2">LEFT(C132,1)</f>
         <v>K</v>
       </c>
       <c r="C132" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D132" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J132" s="1">
         <v>41752</v>
@@ -11360,10 +11666,10 @@
         <v>K</v>
       </c>
       <c r="C133" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D133" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J133" s="1">
         <v>41752</v>
@@ -11378,10 +11684,10 @@
         <v>K</v>
       </c>
       <c r="C134" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D134" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J134" s="1">
         <v>41752</v>
@@ -11396,10 +11702,10 @@
         <v>K</v>
       </c>
       <c r="C135" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D135" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J135" s="1">
         <v>41752</v>
@@ -11414,10 +11720,10 @@
         <v>K</v>
       </c>
       <c r="C136" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D136" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J136" s="1">
         <v>41752</v>
@@ -11432,10 +11738,10 @@
         <v>K</v>
       </c>
       <c r="C137" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D137" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J137" s="1">
         <v>41752</v>
@@ -11450,10 +11756,10 @@
         <v>K</v>
       </c>
       <c r="C138" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D138" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J138" s="1">
         <v>41752</v>
@@ -11468,10 +11774,10 @@
         <v>K</v>
       </c>
       <c r="C139" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D139" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J139" s="1">
         <v>41752</v>
@@ -11486,10 +11792,10 @@
         <v>K</v>
       </c>
       <c r="C140" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D140" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J140" s="1">
         <v>41752</v>
@@ -11501,13 +11807,13 @@
       </c>
       <c r="B141" t="str">
         <f t="shared" si="2"/>
-        <v>L</v>
+        <v>K</v>
       </c>
       <c r="C141" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D141" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J141" s="1">
         <v>41752</v>
@@ -11522,10 +11828,10 @@
         <v>L</v>
       </c>
       <c r="C142" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D142" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J142" s="1">
         <v>41752</v>
@@ -11540,10 +11846,10 @@
         <v>L</v>
       </c>
       <c r="C143" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D143" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J143" s="1">
         <v>41752</v>
@@ -11558,10 +11864,10 @@
         <v>L</v>
       </c>
       <c r="C144" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D144" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J144" s="1">
         <v>41752</v>
@@ -11576,10 +11882,10 @@
         <v>L</v>
       </c>
       <c r="C145" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D145" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J145" s="1">
         <v>41752</v>
@@ -11594,10 +11900,10 @@
         <v>L</v>
       </c>
       <c r="C146" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D146" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J146" s="1">
         <v>41752</v>
@@ -11612,10 +11918,10 @@
         <v>L</v>
       </c>
       <c r="C147" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D147" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J147" s="1">
         <v>41752</v>
@@ -11630,10 +11936,10 @@
         <v>L</v>
       </c>
       <c r="C148" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D148" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J148" s="1">
         <v>41752</v>
@@ -11648,10 +11954,10 @@
         <v>L</v>
       </c>
       <c r="C149" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D149" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J149" s="1">
         <v>41752</v>
@@ -11666,10 +11972,10 @@
         <v>L</v>
       </c>
       <c r="C150" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D150" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J150" s="1">
         <v>41752</v>
@@ -11684,10 +11990,10 @@
         <v>L</v>
       </c>
       <c r="C151" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D151" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J151" s="1">
         <v>41752</v>
@@ -11702,10 +12008,10 @@
         <v>L</v>
       </c>
       <c r="C152" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D152" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J152" s="1">
         <v>41752</v>
@@ -11720,10 +12026,10 @@
         <v>L</v>
       </c>
       <c r="C153" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D153" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J153" s="1">
         <v>41752</v>
@@ -11738,10 +12044,10 @@
         <v>L</v>
       </c>
       <c r="C154" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D154" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J154" s="1">
         <v>41752</v>
@@ -11756,10 +12062,10 @@
         <v>L</v>
       </c>
       <c r="C155" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D155" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J155" s="1">
         <v>41752</v>
@@ -11774,10 +12080,10 @@
         <v>L</v>
       </c>
       <c r="C156" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D156" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J156" s="1">
         <v>41752</v>
@@ -11792,10 +12098,10 @@
         <v>L</v>
       </c>
       <c r="C157" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D157" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J157" s="1">
         <v>41752</v>
@@ -11810,10 +12116,10 @@
         <v>L</v>
       </c>
       <c r="C158" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D158" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J158" s="1">
         <v>41752</v>
@@ -11828,10 +12134,10 @@
         <v>L</v>
       </c>
       <c r="C159" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D159" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J159" s="1">
         <v>41752</v>
@@ -11846,10 +12152,10 @@
         <v>L</v>
       </c>
       <c r="C160" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D160" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J160" s="1">
         <v>41752</v>
@@ -11861,13 +12167,13 @@
       </c>
       <c r="B161" t="str">
         <f t="shared" si="2"/>
-        <v>M</v>
+        <v>L</v>
       </c>
       <c r="C161" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D161" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J161" s="1">
         <v>41752</v>
@@ -11882,10 +12188,10 @@
         <v>M</v>
       </c>
       <c r="C162" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D162" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J162" s="1">
         <v>41752</v>
@@ -11900,10 +12206,10 @@
         <v>M</v>
       </c>
       <c r="C163" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D163" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J163" s="1">
         <v>41752</v>
@@ -11918,10 +12224,10 @@
         <v>M</v>
       </c>
       <c r="C164" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D164" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J164" s="1">
         <v>41752</v>
@@ -11936,10 +12242,10 @@
         <v>M</v>
       </c>
       <c r="C165" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D165" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J165" s="1">
         <v>41752</v>
@@ -11954,10 +12260,10 @@
         <v>M</v>
       </c>
       <c r="C166" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D166" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J166" s="1">
         <v>41752</v>
@@ -11972,10 +12278,10 @@
         <v>M</v>
       </c>
       <c r="C167" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D167" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J167" s="1">
         <v>41752</v>
@@ -11990,10 +12296,10 @@
         <v>M</v>
       </c>
       <c r="C168" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D168" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="J168" s="1">
         <v>41752</v>
@@ -12008,10 +12314,10 @@
         <v>M</v>
       </c>
       <c r="C169" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D169" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="J169" s="1">
         <v>41752</v>
@@ -12026,10 +12332,10 @@
         <v>M</v>
       </c>
       <c r="C170" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D170" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="J170" s="1">
         <v>41752</v>
@@ -12041,13 +12347,13 @@
       </c>
       <c r="B171" t="str">
         <f t="shared" si="2"/>
-        <v>N</v>
+        <v>M</v>
       </c>
       <c r="C171" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D171" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J171" s="1">
         <v>41752</v>
@@ -12062,10 +12368,10 @@
         <v>N</v>
       </c>
       <c r="C172" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D172" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J172" s="1">
         <v>41752</v>
@@ -12080,10 +12386,10 @@
         <v>N</v>
       </c>
       <c r="C173" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D173" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="J173" s="1">
         <v>41752</v>
@@ -12098,10 +12404,10 @@
         <v>N</v>
       </c>
       <c r="C174" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D174" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J174" s="1">
         <v>41752</v>
@@ -12116,10 +12422,10 @@
         <v>N</v>
       </c>
       <c r="C175" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D175" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J175" s="1">
         <v>41752</v>
@@ -12134,10 +12440,10 @@
         <v>N</v>
       </c>
       <c r="C176" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D176" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J176" s="1">
         <v>41752</v>
@@ -12152,10 +12458,10 @@
         <v>N</v>
       </c>
       <c r="C177" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D177" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J177" s="1">
         <v>41752</v>
@@ -12170,10 +12476,10 @@
         <v>N</v>
       </c>
       <c r="C178" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D178" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J178" s="1">
         <v>41752</v>
@@ -12188,10 +12494,10 @@
         <v>N</v>
       </c>
       <c r="C179" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D179" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J179" s="1">
         <v>41752</v>
@@ -12206,10 +12512,10 @@
         <v>N</v>
       </c>
       <c r="C180" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D180" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J180" s="1">
         <v>41752</v>
@@ -12224,10 +12530,10 @@
         <v>N</v>
       </c>
       <c r="C181" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D181" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J181" s="1">
         <v>41752</v>
@@ -12242,10 +12548,10 @@
         <v>N</v>
       </c>
       <c r="C182" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D182" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J182" s="1">
         <v>41752</v>
@@ -12260,10 +12566,10 @@
         <v>N</v>
       </c>
       <c r="C183" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D183" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J183" s="1">
         <v>41752</v>
@@ -12278,10 +12584,10 @@
         <v>N</v>
       </c>
       <c r="C184" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D184" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J184" s="1">
         <v>41752</v>
@@ -12296,10 +12602,10 @@
         <v>N</v>
       </c>
       <c r="C185" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D185" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J185" s="1">
         <v>41752</v>
@@ -12314,10 +12620,10 @@
         <v>N</v>
       </c>
       <c r="C186" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D186" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J186" s="1">
         <v>41752</v>
@@ -12329,13 +12635,13 @@
       </c>
       <c r="B187" t="str">
         <f t="shared" si="2"/>
-        <v>O</v>
+        <v>N</v>
       </c>
       <c r="C187" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D187" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J187" s="1">
         <v>41752</v>
@@ -12350,10 +12656,10 @@
         <v>O</v>
       </c>
       <c r="C188" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D188" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J188" s="1">
         <v>41752</v>
@@ -12368,10 +12674,10 @@
         <v>O</v>
       </c>
       <c r="C189" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D189" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J189" s="1">
         <v>41752</v>
@@ -12386,10 +12692,10 @@
         <v>O</v>
       </c>
       <c r="C190" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D190" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J190" s="1">
         <v>41752</v>
@@ -12404,10 +12710,10 @@
         <v>O</v>
       </c>
       <c r="C191" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D191" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J191" s="1">
         <v>41752</v>
@@ -12422,10 +12728,10 @@
         <v>O</v>
       </c>
       <c r="C192" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D192" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J192" s="1">
         <v>41752</v>
@@ -12440,10 +12746,10 @@
         <v>O</v>
       </c>
       <c r="C193" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D193" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J193" s="1">
         <v>41752</v>
@@ -12458,10 +12764,10 @@
         <v>O</v>
       </c>
       <c r="C194" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D194" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J194" s="1">
         <v>41752</v>
@@ -12472,14 +12778,14 @@
         <v>620</v>
       </c>
       <c r="B195" t="str">
-        <f t="shared" ref="B195:B258" si="3">LEFT(C195,1)</f>
+        <f t="shared" si="2"/>
         <v>O</v>
       </c>
       <c r="C195" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D195" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J195" s="1">
         <v>41752</v>
@@ -12490,14 +12796,14 @@
         <v>620</v>
       </c>
       <c r="B196" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B196:B259" si="3">LEFT(C196,1)</f>
         <v>O</v>
       </c>
       <c r="C196" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D196" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J196" s="1">
         <v>41752</v>
@@ -12512,10 +12818,10 @@
         <v>O</v>
       </c>
       <c r="C197" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D197" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J197" s="1">
         <v>41752</v>
@@ -12530,10 +12836,10 @@
         <v>O</v>
       </c>
       <c r="C198" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D198" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J198" s="1">
         <v>41752</v>
@@ -12548,10 +12854,10 @@
         <v>O</v>
       </c>
       <c r="C199" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D199" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J199" s="1">
         <v>41752</v>
@@ -12566,10 +12872,10 @@
         <v>O</v>
       </c>
       <c r="C200" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D200" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J200" s="1">
         <v>41752</v>
@@ -12584,10 +12890,10 @@
         <v>O</v>
       </c>
       <c r="C201" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D201" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J201" s="1">
         <v>41752</v>
@@ -12599,13 +12905,13 @@
       </c>
       <c r="B202" t="str">
         <f t="shared" si="3"/>
-        <v>P</v>
+        <v>O</v>
       </c>
       <c r="C202" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D202" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J202" s="1">
         <v>41752</v>
@@ -12620,10 +12926,10 @@
         <v>P</v>
       </c>
       <c r="C203" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D203" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="J203" s="1">
         <v>41752</v>
@@ -12638,10 +12944,10 @@
         <v>P</v>
       </c>
       <c r="C204" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D204" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J204" s="1">
         <v>41752</v>
@@ -12656,10 +12962,10 @@
         <v>P</v>
       </c>
       <c r="C205" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D205" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J205" s="1">
         <v>41752</v>
@@ -12674,10 +12980,10 @@
         <v>P</v>
       </c>
       <c r="C206" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D206" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J206" s="1">
         <v>41752</v>
@@ -12692,10 +12998,10 @@
         <v>P</v>
       </c>
       <c r="C207" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D207" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J207" s="1">
         <v>41752</v>
@@ -12710,10 +13016,10 @@
         <v>P</v>
       </c>
       <c r="C208" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D208" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J208" s="1">
         <v>41752</v>
@@ -12728,10 +13034,10 @@
         <v>P</v>
       </c>
       <c r="C209" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D209" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="J209" s="1">
         <v>41752</v>
@@ -12746,10 +13052,10 @@
         <v>P</v>
       </c>
       <c r="C210" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D210" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J210" s="1">
         <v>41752</v>
@@ -12764,10 +13070,10 @@
         <v>P</v>
       </c>
       <c r="C211" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D211" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J211" s="1">
         <v>41752</v>
@@ -12782,10 +13088,10 @@
         <v>P</v>
       </c>
       <c r="C212" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D212" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J212" s="1">
         <v>41752</v>
@@ -12800,10 +13106,10 @@
         <v>P</v>
       </c>
       <c r="C213" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D213" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J213" s="1">
         <v>41752</v>
@@ -12818,10 +13124,10 @@
         <v>P</v>
       </c>
       <c r="C214" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D214" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J214" s="1">
         <v>41752</v>
@@ -12836,10 +13142,10 @@
         <v>P</v>
       </c>
       <c r="C215" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D215" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J215" s="1">
         <v>41752</v>
@@ -12854,10 +13160,10 @@
         <v>P</v>
       </c>
       <c r="C216" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D216" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J216" s="1">
         <v>41752</v>
@@ -12872,10 +13178,10 @@
         <v>P</v>
       </c>
       <c r="C217" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D217" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J217" s="1">
         <v>41752</v>
@@ -12890,10 +13196,10 @@
         <v>P</v>
       </c>
       <c r="C218" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D218" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J218" s="1">
         <v>41752</v>
@@ -12908,10 +13214,10 @@
         <v>P</v>
       </c>
       <c r="C219" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D219" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J219" s="1">
         <v>41752</v>
@@ -12926,10 +13232,10 @@
         <v>P</v>
       </c>
       <c r="C220" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D220" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J220" s="1">
         <v>41752</v>
@@ -12944,10 +13250,10 @@
         <v>P</v>
       </c>
       <c r="C221" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D221" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J221" s="1">
         <v>41752</v>
@@ -12962,10 +13268,10 @@
         <v>P</v>
       </c>
       <c r="C222" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D222" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J222" s="1">
         <v>41752</v>
@@ -12980,10 +13286,10 @@
         <v>P</v>
       </c>
       <c r="C223" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D223" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J223" s="1">
         <v>41752</v>
@@ -12998,10 +13304,10 @@
         <v>P</v>
       </c>
       <c r="C224" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D224" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J224" s="1">
         <v>41752</v>
@@ -13016,10 +13322,10 @@
         <v>P</v>
       </c>
       <c r="C225" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D225" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J225" s="1">
         <v>41752</v>
@@ -13034,10 +13340,10 @@
         <v>P</v>
       </c>
       <c r="C226" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D226" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J226" s="1">
         <v>41752</v>
@@ -13049,13 +13355,13 @@
       </c>
       <c r="B227" t="str">
         <f t="shared" si="3"/>
-        <v>R</v>
+        <v>P</v>
       </c>
       <c r="C227" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D227" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J227" s="1">
         <v>41752</v>
@@ -13070,10 +13376,10 @@
         <v>R</v>
       </c>
       <c r="C228" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D228" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="J228" s="1">
         <v>41752</v>
@@ -13088,10 +13394,10 @@
         <v>R</v>
       </c>
       <c r="C229" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D229" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J229" s="1">
         <v>41752</v>
@@ -13106,10 +13412,10 @@
         <v>R</v>
       </c>
       <c r="C230" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D230" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J230" s="1">
         <v>41752</v>
@@ -13124,10 +13430,10 @@
         <v>R</v>
       </c>
       <c r="C231" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D231" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J231" s="1">
         <v>41752</v>
@@ -13139,13 +13445,13 @@
       </c>
       <c r="B232" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>R</v>
       </c>
       <c r="C232" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D232" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J232" s="1">
         <v>41752</v>
@@ -13160,10 +13466,10 @@
         <v>S</v>
       </c>
       <c r="C233" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D233" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J233" s="1">
         <v>41752</v>
@@ -13178,10 +13484,10 @@
         <v>S</v>
       </c>
       <c r="C234" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D234" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J234" s="1">
         <v>41752</v>
@@ -13196,10 +13502,10 @@
         <v>S</v>
       </c>
       <c r="C235" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D235" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J235" s="1">
         <v>41752</v>
@@ -13214,10 +13520,10 @@
         <v>S</v>
       </c>
       <c r="C236" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D236" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J236" s="1">
         <v>41752</v>
@@ -13232,10 +13538,10 @@
         <v>S</v>
       </c>
       <c r="C237" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D237" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J237" s="1">
         <v>41752</v>
@@ -13250,10 +13556,10 @@
         <v>S</v>
       </c>
       <c r="C238" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D238" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="J238" s="1">
         <v>41752</v>
@@ -13268,10 +13574,10 @@
         <v>S</v>
       </c>
       <c r="C239" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D239" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J239" s="1">
         <v>41752</v>
@@ -13286,10 +13592,10 @@
         <v>S</v>
       </c>
       <c r="C240" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D240" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J240" s="1">
         <v>41752</v>
@@ -13304,10 +13610,10 @@
         <v>S</v>
       </c>
       <c r="C241" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D241" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J241" s="1">
         <v>41752</v>
@@ -13322,10 +13628,10 @@
         <v>S</v>
       </c>
       <c r="C242" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D242" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J242" s="1">
         <v>41752</v>
@@ -13340,10 +13646,10 @@
         <v>S</v>
       </c>
       <c r="C243" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D243" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="J243" s="1">
         <v>41752</v>
@@ -13358,10 +13664,10 @@
         <v>S</v>
       </c>
       <c r="C244" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D244" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J244" s="1">
         <v>41752</v>
@@ -13376,10 +13682,10 @@
         <v>S</v>
       </c>
       <c r="C245" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D245" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J245" s="1">
         <v>41752</v>
@@ -13394,10 +13700,10 @@
         <v>S</v>
       </c>
       <c r="C246" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D246" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J246" s="1">
         <v>41752</v>
@@ -13412,10 +13718,10 @@
         <v>S</v>
       </c>
       <c r="C247" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D247" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J247" s="1">
         <v>41752</v>
@@ -13430,10 +13736,10 @@
         <v>S</v>
       </c>
       <c r="C248" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D248" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J248" s="1">
         <v>41752</v>
@@ -13448,10 +13754,10 @@
         <v>S</v>
       </c>
       <c r="C249" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D249" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="J249" s="1">
         <v>41752</v>
@@ -13466,10 +13772,10 @@
         <v>S</v>
       </c>
       <c r="C250" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D250" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="J250" s="1">
         <v>41752</v>
@@ -13484,10 +13790,10 @@
         <v>S</v>
       </c>
       <c r="C251" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D251" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="J251" s="1">
         <v>41752</v>
@@ -13502,10 +13808,10 @@
         <v>S</v>
       </c>
       <c r="C252" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D252" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="J252" s="1">
         <v>41752</v>
@@ -13520,10 +13826,10 @@
         <v>S</v>
       </c>
       <c r="C253" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D253" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="J253" s="1">
         <v>41752</v>
@@ -13538,10 +13844,10 @@
         <v>S</v>
       </c>
       <c r="C254" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D254" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="J254" s="1">
         <v>41752</v>
@@ -13553,13 +13859,13 @@
       </c>
       <c r="B255" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="C255" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D255" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J255" s="1">
         <v>41752</v>
@@ -13574,10 +13880,10 @@
         <v>T</v>
       </c>
       <c r="C256" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D256" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J256" s="1">
         <v>41752</v>
@@ -13592,10 +13898,10 @@
         <v>T</v>
       </c>
       <c r="C257" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D257" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J257" s="1">
         <v>41752</v>
@@ -13610,10 +13916,10 @@
         <v>T</v>
       </c>
       <c r="C258" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D258" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="J258" s="1">
         <v>41752</v>
@@ -13624,14 +13930,14 @@
         <v>620</v>
       </c>
       <c r="B259" t="str">
-        <f t="shared" ref="B259:B311" si="4">LEFT(C259,1)</f>
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
       <c r="C259" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D259" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J259" s="1">
         <v>41752</v>
@@ -13642,14 +13948,14 @@
         <v>620</v>
       </c>
       <c r="B260" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B260:B312" si="4">LEFT(C260,1)</f>
         <v>T</v>
       </c>
       <c r="C260" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D260" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J260" s="1">
         <v>41752</v>
@@ -13664,10 +13970,10 @@
         <v>T</v>
       </c>
       <c r="C261" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D261" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J261" s="1">
         <v>41752</v>
@@ -13682,10 +13988,10 @@
         <v>T</v>
       </c>
       <c r="C262" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D262" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="J262" s="1">
         <v>41752</v>
@@ -13700,10 +14006,10 @@
         <v>T</v>
       </c>
       <c r="C263" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D263" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="J263" s="1">
         <v>41752</v>
@@ -13718,10 +14024,10 @@
         <v>T</v>
       </c>
       <c r="C264" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D264" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="J264" s="1">
         <v>41752</v>
@@ -13736,10 +14042,10 @@
         <v>T</v>
       </c>
       <c r="C265" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D265" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="J265" s="1">
         <v>41752</v>
@@ -13754,10 +14060,10 @@
         <v>T</v>
       </c>
       <c r="C266" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D266" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J266" s="1">
         <v>41752</v>
@@ -13772,10 +14078,10 @@
         <v>T</v>
       </c>
       <c r="C267" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D267" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="J267" s="1">
         <v>41752</v>
@@ -13790,10 +14096,10 @@
         <v>T</v>
       </c>
       <c r="C268" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D268" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J268" s="1">
         <v>41752</v>
@@ -13808,10 +14114,10 @@
         <v>T</v>
       </c>
       <c r="C269" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D269" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J269" s="1">
         <v>41752</v>
@@ -13826,10 +14132,10 @@
         <v>T</v>
       </c>
       <c r="C270" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D270" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="J270" s="1">
         <v>41752</v>
@@ -13844,10 +14150,10 @@
         <v>T</v>
       </c>
       <c r="C271" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D271" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J271" s="1">
         <v>41752</v>
@@ -13862,10 +14168,10 @@
         <v>T</v>
       </c>
       <c r="C272" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D272" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="J272" s="1">
         <v>41752</v>
@@ -13880,10 +14186,10 @@
         <v>T</v>
       </c>
       <c r="C273" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D273" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="J273" s="1">
         <v>41752</v>
@@ -13898,10 +14204,10 @@
         <v>T</v>
       </c>
       <c r="C274" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D274" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="J274" s="1">
         <v>41752</v>
@@ -13916,10 +14222,10 @@
         <v>T</v>
       </c>
       <c r="C275" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D275" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J275" s="1">
         <v>41752</v>
@@ -13934,10 +14240,10 @@
         <v>T</v>
       </c>
       <c r="C276" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D276" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J276" s="1">
         <v>41752</v>
@@ -13952,10 +14258,10 @@
         <v>T</v>
       </c>
       <c r="C277" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D277" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J277" s="1">
         <v>41752</v>
@@ -13970,10 +14276,10 @@
         <v>T</v>
       </c>
       <c r="C278" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D278" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="J278" s="1">
         <v>41752</v>
@@ -13988,10 +14294,10 @@
         <v>T</v>
       </c>
       <c r="C279" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D279" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J279" s="1">
         <v>41752</v>
@@ -14006,10 +14312,10 @@
         <v>T</v>
       </c>
       <c r="C280" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D280" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="J280" s="1">
         <v>41752</v>
@@ -14024,10 +14330,10 @@
         <v>T</v>
       </c>
       <c r="C281" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D281" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J281" s="1">
         <v>41752</v>
@@ -14042,10 +14348,10 @@
         <v>T</v>
       </c>
       <c r="C282" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D282" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="J282" s="1">
         <v>41752</v>
@@ -14060,10 +14366,10 @@
         <v>T</v>
       </c>
       <c r="C283" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D283" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="J283" s="1">
         <v>41752</v>
@@ -14075,13 +14381,13 @@
       </c>
       <c r="B284" t="str">
         <f t="shared" si="4"/>
-        <v>U</v>
+        <v>T</v>
       </c>
       <c r="C284" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D284" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="J284" s="1">
         <v>41752</v>
@@ -14096,10 +14402,10 @@
         <v>U</v>
       </c>
       <c r="C285" t="s">
-        <v>61</v>
+        <v>568</v>
       </c>
       <c r="D285" t="s">
-        <v>60</v>
+        <v>569</v>
       </c>
       <c r="J285" s="1">
         <v>41752</v>
@@ -14114,10 +14420,10 @@
         <v>U</v>
       </c>
       <c r="C286" t="s">
-        <v>570</v>
+        <v>61</v>
       </c>
       <c r="D286" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="J286" s="1">
         <v>41752</v>
@@ -14132,10 +14438,10 @@
         <v>U</v>
       </c>
       <c r="C287" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D287" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="J287" s="1">
         <v>41752</v>
@@ -14150,10 +14456,10 @@
         <v>U</v>
       </c>
       <c r="C288" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D288" t="s">
-        <v>573</v>
+        <v>169</v>
       </c>
       <c r="J288" s="1">
         <v>41752</v>
@@ -14168,10 +14474,10 @@
         <v>U</v>
       </c>
       <c r="C289" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D289" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J289" s="1">
         <v>41752</v>
@@ -14186,10 +14492,10 @@
         <v>U</v>
       </c>
       <c r="C290" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D290" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="J290" s="1">
         <v>41752</v>
@@ -14204,10 +14510,10 @@
         <v>U</v>
       </c>
       <c r="C291" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D291" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="J291" s="1">
         <v>41752</v>
@@ -14222,10 +14528,10 @@
         <v>U</v>
       </c>
       <c r="C292" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D292" t="s">
-        <v>335</v>
+        <v>579</v>
       </c>
       <c r="J292" s="1">
         <v>41752</v>
@@ -14240,10 +14546,10 @@
         <v>U</v>
       </c>
       <c r="C293" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D293" t="s">
-        <v>582</v>
+        <v>335</v>
       </c>
       <c r="J293" s="1">
         <v>41752</v>
@@ -14258,10 +14564,10 @@
         <v>U</v>
       </c>
       <c r="C294" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D294" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J294" s="1">
         <v>41752</v>
@@ -14276,10 +14582,10 @@
         <v>U</v>
       </c>
       <c r="C295" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D295" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J295" s="1">
         <v>41752</v>
@@ -14294,10 +14600,10 @@
         <v>U</v>
       </c>
       <c r="C296" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D296" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J296" s="1">
         <v>41752</v>
@@ -14312,10 +14618,10 @@
         <v>U</v>
       </c>
       <c r="C297" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D297" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="J297" s="1">
         <v>41752</v>
@@ -14330,10 +14636,10 @@
         <v>U</v>
       </c>
       <c r="C298" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D298" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="J298" s="1">
         <v>41752</v>
@@ -14348,10 +14654,10 @@
         <v>U</v>
       </c>
       <c r="C299" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D299" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J299" s="1">
         <v>41752</v>
@@ -14366,10 +14672,10 @@
         <v>U</v>
       </c>
       <c r="C300" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D300" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="J300" s="1">
         <v>41752</v>
@@ -14384,10 +14690,10 @@
         <v>U</v>
       </c>
       <c r="C301" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D301" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J301" s="1">
         <v>41752</v>
@@ -14399,13 +14705,13 @@
       </c>
       <c r="B302" t="str">
         <f t="shared" si="4"/>
-        <v>V</v>
+        <v>U</v>
       </c>
       <c r="C302" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D302" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="J302" s="1">
         <v>41752</v>
@@ -14420,10 +14726,10 @@
         <v>V</v>
       </c>
       <c r="C303" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D303" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J303" s="1">
         <v>41752</v>
@@ -14438,10 +14744,10 @@
         <v>V</v>
       </c>
       <c r="C304" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D304" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J304" s="1">
         <v>41752</v>
@@ -14456,10 +14762,10 @@
         <v>V</v>
       </c>
       <c r="C305" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D305" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="J305" s="1">
         <v>41752</v>
@@ -14474,10 +14780,10 @@
         <v>V</v>
       </c>
       <c r="C306" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D306" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J306" s="1">
         <v>41752</v>
@@ -14492,10 +14798,10 @@
         <v>V</v>
       </c>
       <c r="C307" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D307" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="J307" s="1">
         <v>41752</v>
@@ -14510,10 +14816,10 @@
         <v>V</v>
       </c>
       <c r="C308" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D308" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J308" s="1">
         <v>41752</v>
@@ -14528,10 +14834,10 @@
         <v>V</v>
       </c>
       <c r="C309" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D309" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J309" s="1">
         <v>41752</v>
@@ -14543,13 +14849,13 @@
       </c>
       <c r="B310" t="str">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v>V</v>
       </c>
       <c r="C310" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D310" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="J310" s="1">
         <v>41752</v>
@@ -14561,22 +14867,42 @@
       </c>
       <c r="B311" t="str">
         <f t="shared" si="4"/>
+        <v>X</v>
+      </c>
+      <c r="C311" t="s">
+        <v>615</v>
+      </c>
+      <c r="D311" t="s">
+        <v>616</v>
+      </c>
+      <c r="J311" s="1">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>620</v>
+      </c>
+      <c r="B312" t="str">
+        <f t="shared" si="4"/>
         <v>Y</v>
       </c>
-      <c r="C311" t="s">
+      <c r="C312" t="s">
         <v>617</v>
       </c>
-      <c r="D311" t="s">
+      <c r="D312" t="s">
         <v>618</v>
       </c>
-      <c r="J311" s="1">
+      <c r="J312" s="1">
         <v>41752</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M311">
+  <autoFilter ref="A1:M312">
     <filterColumn colId="5">
-      <filters blank="1"/>
+      <filters blank="1">
+        <filter val="OK"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed items that where accidently removed and added L group
</commit_message>
<xml_diff>
--- a/snomed/volven-8352-snomed.xlsx
+++ b/snomed/volven-8352-snomed.xlsx
@@ -20,13 +20,13 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="907">
   <si>
     <t>Kode</t>
   </si>
@@ -2642,6 +2642,111 @@
   </si>
   <si>
     <t>Kolonneetiketter</t>
+  </si>
+  <si>
+    <t>74670003 | Wrist joint structure (body structure)</t>
+  </si>
+  <si>
+    <t>41695006 | Scalp structure (body structure)</t>
+  </si>
+  <si>
+    <t>29836001 | Hip region structure (body structure)</t>
+  </si>
+  <si>
+    <t>29850006 | Iliac crest structure (body structure)</t>
+  </si>
+  <si>
+    <t>24136001 | Hip joint structure (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39937001 | Skin structure (body structure) </t>
+  </si>
+  <si>
+    <t>34516001 | Ileal structure (body structure)</t>
+  </si>
+  <si>
+    <t>182321004 | Crown of head (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18857001 | Vaginal introitus structure (body structure) </t>
+  </si>
+  <si>
+    <t>21306003 | Jejunal structure (body structure)</t>
+  </si>
+  <si>
+    <t>60819002 | Cheek structure (body structure)</t>
+  </si>
+  <si>
+    <t>661005 | Jaw region structure (body structure)</t>
+  </si>
+  <si>
+    <t>65439009 | Clitoral structure (body structure)</t>
+  </si>
+  <si>
+    <t>72696002 | Knee region structure (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6902008 | Popliteal region structure (body structure) </t>
+  </si>
+  <si>
+    <t>49076000 | Knee joint structure (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">421413000 | Structure of patella (body structure) </t>
+  </si>
+  <si>
+    <t>37822005 | Lower back structure (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4596009 | Laryngeal structure (body structure) </t>
+  </si>
+  <si>
+    <t>10200004 | Liver structure (body structure)</t>
+  </si>
+  <si>
+    <t>39352004 | Joint structure (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53840002 | Structure of calf of leg (body structure) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">48477009 | Lip structure (body structure) </t>
+  </si>
+  <si>
+    <t>Kan også gjelde lepper generelt, men dette er for lepper i ansiktet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29627003 | Structure of neck of femur (body structure) </t>
+  </si>
+  <si>
+    <t>82462005 | Labium majus structure (body structure)</t>
+  </si>
+  <si>
+    <t>32104003 | Labium minus structure (body structure)</t>
+  </si>
+  <si>
+    <t>68367000 | Thigh structure (body structure)</t>
+  </si>
+  <si>
+    <t>26893007 | Inguinal region structure (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39607008 | Lung structure (body structure) </t>
+  </si>
+  <si>
+    <t>40020002 | Structure of middle lobe of lung (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45653009 | Structure of upper lobe of lung (body structure) </t>
+  </si>
+  <si>
+    <t>90572001 | Structure of lower lobe of lung (body structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hva er forskjell på lyske og lyskregion ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">52612000 | Lumbar region back structure (body structure) </t>
   </si>
 </sst>
 </file>
@@ -3226,8 +3331,1121 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nb-NO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[volven-8352-snomed.xlsx]Ark2!Pivottabell3</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark2'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GRUPPE1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ark2'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>NOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OK</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UKLAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>USIKKER</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(tom)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark2'!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark2'!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GRUPPE2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ark2'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>NOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OK</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UKLAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>USIKKER</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(tom)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark2'!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark2'!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(tom)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ark2'!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>NOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OK</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UKLAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>USIKKER</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(tom)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark2'!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="100"/>
+        <c:axId val="416943280"/>
+        <c:axId val="416944064"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="416943280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="416944064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="416944064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="416943280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723901</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Bjørn Næss" refreshedDate="42660.288137731484" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="311">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Bjørn Næss" refreshedDate="42660.446668750003" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="311">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N312" sheet="Anatomisk lokalisasjon"/>
   </cacheSource>
@@ -5105,8 +6323,8 @@
     <s v="H"/>
     <s v="HL"/>
     <s v="Håndledd"/>
-    <m/>
-    <x v="4"/>
+    <s v="74670003 | Wrist joint structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5137,8 +6355,8 @@
     <s v="H"/>
     <s v="HOB"/>
     <s v="Hodebunn"/>
-    <m/>
-    <x v="4"/>
+    <s v="41695006 | Scalp structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5169,8 +6387,8 @@
     <s v="H"/>
     <s v="HOF"/>
     <s v="Hofte"/>
-    <m/>
-    <x v="4"/>
+    <s v="29836001 | Hip region structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5185,8 +6403,8 @@
     <s v="H"/>
     <s v="HOK"/>
     <s v="Hoftekam"/>
-    <m/>
-    <x v="4"/>
+    <s v="29850006 | Iliac crest structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5201,8 +6419,8 @@
     <s v="H"/>
     <s v="HOL"/>
     <s v="Hofteledd"/>
-    <m/>
-    <x v="4"/>
+    <s v="24136001 | Hip joint structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5218,7 +6436,7 @@
     <s v="HOP"/>
     <s v="Hofteprotese"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5233,8 +6451,8 @@
     <s v="H"/>
     <s v="HUD"/>
     <s v="Hud"/>
-    <m/>
-    <x v="4"/>
+    <s v="39937001 | Skin structure (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5250,7 +6468,7 @@
     <s v="ICR"/>
     <s v="Intracranielt"/>
     <m/>
-    <x v="4"/>
+    <x v="3"/>
     <m/>
     <m/>
     <m/>
@@ -5265,8 +6483,8 @@
     <s v="I"/>
     <s v="IL"/>
     <s v="Ileum"/>
-    <m/>
-    <x v="4"/>
+    <s v="34516001 | Ileal structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5282,7 +6500,7 @@
     <s v="INS"/>
     <s v="Innstikkssted"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5297,8 +6515,8 @@
     <s v="I"/>
     <s v="ISS"/>
     <s v="Isse"/>
-    <m/>
-    <x v="4"/>
+    <s v="182321004 | Crown of head (body structure)"/>
+    <x v="2"/>
     <m/>
     <m/>
     <m/>
@@ -5313,8 +6531,8 @@
     <s v="I"/>
     <s v="IVA"/>
     <s v="Introitus vaginae"/>
-    <m/>
-    <x v="4"/>
+    <s v="18857001 | Vaginal introitus structure (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5329,8 +6547,8 @@
     <s v="J"/>
     <s v="JE"/>
     <s v="Jejunum"/>
-    <m/>
-    <x v="4"/>
+    <s v="21306003 | Jejunal structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5346,7 +6564,7 @@
     <s v="KAE"/>
     <s v="Kateter engangs"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5362,7 +6580,7 @@
     <s v="KAI"/>
     <s v="Kateter innleggelse"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5378,7 +6596,7 @@
     <s v="KAP"/>
     <s v="Kateter permanent"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5394,7 +6612,7 @@
     <s v="KAT"/>
     <s v="Kateter"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5409,8 +6627,8 @@
     <s v="K"/>
     <s v="KIN"/>
     <s v="Kinn"/>
-    <m/>
-    <x v="4"/>
+    <s v="60819002 | Cheek structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5425,8 +6643,8 @@
     <s v="K"/>
     <s v="KJE"/>
     <s v="Kjeve"/>
-    <m/>
-    <x v="4"/>
+    <s v="661005 | Jaw region structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5441,8 +6659,8 @@
     <s v="K"/>
     <s v="KLI"/>
     <s v="Klitoris"/>
-    <m/>
-    <x v="4"/>
+    <s v="65439009 | Clitoral structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5457,8 +6675,8 @@
     <s v="K"/>
     <s v="KNE"/>
     <s v="Kne"/>
-    <m/>
-    <x v="4"/>
+    <s v="72696002 | Knee region structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5473,8 +6691,8 @@
     <s v="K"/>
     <s v="KNH"/>
     <s v="Knehase"/>
-    <m/>
-    <x v="4"/>
+    <s v="6902008 | Popliteal region structure (body structure) "/>
+    <x v="2"/>
     <m/>
     <m/>
     <m/>
@@ -5489,8 +6707,8 @@
     <s v="K"/>
     <s v="KNL"/>
     <s v="Kneledd"/>
-    <m/>
-    <x v="4"/>
+    <s v="49076000 | Knee joint structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5506,7 +6724,7 @@
     <s v="KNP"/>
     <s v="Kneprotese"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5521,8 +6739,8 @@
     <s v="K"/>
     <s v="KNS"/>
     <s v="Kneskål"/>
-    <m/>
-    <x v="4"/>
+    <s v="421413000 | Structure of patella (body structure) "/>
+    <x v="2"/>
     <m/>
     <m/>
     <m/>
@@ -5537,8 +6755,8 @@
     <s v="K"/>
     <s v="KOR"/>
     <s v="Korsrygg"/>
-    <m/>
-    <x v="4"/>
+    <s v="37822005 | Lower back structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5553,8 +6771,8 @@
     <s v="L"/>
     <s v="LAR"/>
     <s v="Larynx"/>
-    <m/>
-    <x v="4"/>
+    <s v="4596009 | Laryngeal structure (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5569,8 +6787,8 @@
     <s v="L"/>
     <s v="LE"/>
     <s v="Lever"/>
-    <m/>
-    <x v="4"/>
+    <s v="10200004 | Liver structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5585,8 +6803,8 @@
     <s v="L"/>
     <s v="LED"/>
     <s v="Ledd"/>
-    <m/>
-    <x v="4"/>
+    <s v="39352004 | Joint structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5601,8 +6819,8 @@
     <s v="L"/>
     <s v="LEG"/>
     <s v="Legg"/>
-    <m/>
-    <x v="4"/>
+    <s v="53840002 | Structure of calf of leg (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5618,7 +6836,7 @@
     <s v="LEL"/>
     <s v="Leverlapp"/>
     <m/>
-    <x v="4"/>
+    <x v="3"/>
     <m/>
     <m/>
     <m/>
@@ -5633,10 +6851,10 @@
     <s v="L"/>
     <s v="LEP"/>
     <s v="Leppe"/>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <m/>
+    <s v="48477009 | Lip structure (body structure) "/>
+    <x v="0"/>
+    <m/>
+    <s v="Kan også gjelde lepper generelt, men dette er for lepper i ansiktet"/>
     <m/>
     <d v="2014-04-23T00:00:00"/>
     <m/>
@@ -5650,7 +6868,7 @@
     <s v="LES"/>
     <s v="Leggsår"/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -5665,8 +6883,8 @@
     <s v="L"/>
     <s v="LHA"/>
     <s v="Lårhals"/>
-    <m/>
-    <x v="4"/>
+    <s v="29627003 | Structure of neck of femur (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5682,7 +6900,7 @@
     <s v="LIN"/>
     <s v="Linse"/>
     <m/>
-    <x v="4"/>
+    <x v="3"/>
     <m/>
     <m/>
     <m/>
@@ -5697,8 +6915,8 @@
     <s v="L"/>
     <s v="LMA"/>
     <s v="Labium majus"/>
-    <m/>
-    <x v="4"/>
+    <s v="82462005 | Labium majus structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5713,8 +6931,8 @@
     <s v="L"/>
     <s v="LMI"/>
     <s v="Labium minus"/>
-    <m/>
-    <x v="4"/>
+    <s v="32104003 | Labium minus structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5730,7 +6948,7 @@
     <s v="LOK"/>
     <s v="Hud, multiple lokalisasjoner"/>
     <m/>
-    <x v="4"/>
+    <x v="3"/>
     <m/>
     <m/>
     <m/>
@@ -5745,8 +6963,8 @@
     <s v="L"/>
     <s v="LR"/>
     <s v="Lår"/>
-    <m/>
-    <x v="4"/>
+    <s v="68367000 | Thigh structure (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5761,8 +6979,8 @@
     <s v="L"/>
     <s v="LRE"/>
     <s v="Lyskeregion"/>
-    <m/>
-    <x v="4"/>
+    <s v="26893007 | Inguinal region structure (body structure)"/>
+    <x v="2"/>
     <m/>
     <m/>
     <m/>
@@ -5777,8 +6995,8 @@
     <s v="L"/>
     <s v="LU"/>
     <s v="Lunge"/>
-    <m/>
-    <x v="4"/>
+    <s v="39607008 | Lung structure (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5793,8 +7011,8 @@
     <s v="L"/>
     <s v="LUI"/>
     <s v="Lunge, midtlapp"/>
-    <m/>
-    <x v="4"/>
+    <s v="40020002 | Structure of middle lobe of lung (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5809,8 +7027,8 @@
     <s v="L"/>
     <s v="LUM"/>
     <s v="Lumbalregion"/>
-    <m/>
-    <x v="4"/>
+    <s v="52612000 | Lumbar region back structure (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5825,8 +7043,8 @@
     <s v="L"/>
     <s v="LUO"/>
     <s v="Lunge, overlapp"/>
-    <m/>
-    <x v="4"/>
+    <s v="45653009 | Structure of upper lobe of lung (body structure) "/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5841,8 +7059,8 @@
     <s v="L"/>
     <s v="LUU"/>
     <s v="Lunge, underlapp"/>
-    <m/>
-    <x v="4"/>
+    <s v="90572001 | Structure of lower lobe of lung (body structure)"/>
+    <x v="0"/>
     <m/>
     <m/>
     <m/>
@@ -5857,10 +7075,10 @@
     <s v="L"/>
     <s v="LYS"/>
     <s v="Lyske"/>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <m/>
+    <s v="26893007 | Inguinal region structure (body structure)"/>
+    <x v="2"/>
+    <m/>
+    <s v="Hva er forskjell på lyske og lyskregion ? "/>
     <m/>
     <d v="2014-04-23T00:00:00"/>
     <m/>
@@ -8288,15 +9506,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabell3" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Verdier" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivottabell3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Verdier" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="A3:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="19">
         <item m="1" x="8"/>
         <item m="1" x="7"/>
@@ -8326,7 +9544,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="2"/>
@@ -8336,26 +9554,9 @@
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="13"/>
+    <field x="5"/>
   </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="5"/>
-  </colFields>
-  <colItems count="6">
+  <rowItems count="6">
     <i>
       <x v="9"/>
     </i>
@@ -8374,10 +9575,98 @@
     <i t="grand">
       <x/>
     </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="13"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </colItems>
   <dataFields count="1">
     <dataField name="Antall av Kodeverk" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -8650,19 +9939,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G8"/>
+  <dimension ref="A3:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.25" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.5" bestFit="1" customWidth="1"/>
@@ -8678,7 +9967,7 @@
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>742</v>
       </c>
@@ -8686,113 +9975,124 @@
         <v>871</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>648</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>740</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>650</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>674</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>669</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>741</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>739</v>
-      </c>
       <c r="B5" s="4">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C5" s="4">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4">
-        <v>14</v>
-      </c>
-      <c r="F5" s="4">
-        <v>27</v>
-      </c>
-      <c r="G5" s="4">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>740</v>
+        <v>650</v>
       </c>
       <c r="B6" s="4">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="C6" s="4">
         <v>107</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>14</v>
+      </c>
       <c r="E6" s="4">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B7" s="4">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="B8" s="4">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4">
         <v>13</v>
       </c>
-      <c r="F6" s="4">
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="4">
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B10" s="4">
+        <v>139</v>
+      </c>
+      <c r="C10" s="4">
         <v>151</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4">
+      <c r="D10" s="4">
         <v>20</v>
       </c>
-      <c r="G7" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="B8" s="4">
-        <v>45</v>
-      </c>
-      <c r="C8" s="4">
-        <v>175</v>
-      </c>
-      <c r="D8" s="4">
-        <v>15</v>
-      </c>
-      <c r="E8" s="4">
-        <v>27</v>
-      </c>
-      <c r="F8" s="4">
-        <v>48</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="E10" s="4">
         <v>310</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8800,11 +10100,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N312"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11873,6 +13173,12 @@
       <c r="D114" t="s">
         <v>227</v>
       </c>
+      <c r="E114" t="s">
+        <v>872</v>
+      </c>
+      <c r="F114" t="s">
+        <v>650</v>
+      </c>
       <c r="J114" s="1">
         <v>41752</v>
       </c>
@@ -11921,6 +13227,12 @@
       <c r="D116" t="s">
         <v>231</v>
       </c>
+      <c r="E116" t="s">
+        <v>873</v>
+      </c>
+      <c r="F116" t="s">
+        <v>650</v>
+      </c>
       <c r="J116" s="1">
         <v>41752</v>
       </c>
@@ -11969,6 +13281,12 @@
       <c r="D118" t="s">
         <v>235</v>
       </c>
+      <c r="E118" t="s">
+        <v>874</v>
+      </c>
+      <c r="F118" t="s">
+        <v>716</v>
+      </c>
       <c r="J118" s="1">
         <v>41752</v>
       </c>
@@ -11990,6 +13308,12 @@
       <c r="D119" t="s">
         <v>237</v>
       </c>
+      <c r="E119" t="s">
+        <v>875</v>
+      </c>
+      <c r="F119" t="s">
+        <v>650</v>
+      </c>
       <c r="J119" s="1">
         <v>41752</v>
       </c>
@@ -12011,6 +13335,12 @@
       <c r="D120" t="s">
         <v>239</v>
       </c>
+      <c r="E120" t="s">
+        <v>876</v>
+      </c>
+      <c r="F120" t="s">
+        <v>716</v>
+      </c>
       <c r="J120" s="1">
         <v>41752</v>
       </c>
@@ -12032,6 +13362,9 @@
       <c r="D121" t="s">
         <v>241</v>
       </c>
+      <c r="F121" t="s">
+        <v>634</v>
+      </c>
       <c r="J121" s="1">
         <v>41752</v>
       </c>
@@ -12053,6 +13386,12 @@
       <c r="D122" t="s">
         <v>243</v>
       </c>
+      <c r="E122" t="s">
+        <v>877</v>
+      </c>
+      <c r="F122" t="s">
+        <v>650</v>
+      </c>
       <c r="J122" s="1">
         <v>41752</v>
       </c>
@@ -12074,6 +13413,9 @@
       <c r="D123" t="s">
         <v>245</v>
       </c>
+      <c r="F123" t="s">
+        <v>674</v>
+      </c>
       <c r="J123" s="1">
         <v>41752</v>
       </c>
@@ -12095,6 +13437,12 @@
       <c r="D124" t="s">
         <v>247</v>
       </c>
+      <c r="E124" t="s">
+        <v>878</v>
+      </c>
+      <c r="F124" t="s">
+        <v>650</v>
+      </c>
       <c r="J124" s="1">
         <v>41752</v>
       </c>
@@ -12116,6 +13464,9 @@
       <c r="D125" t="s">
         <v>249</v>
       </c>
+      <c r="F125" t="s">
+        <v>634</v>
+      </c>
       <c r="J125" s="1">
         <v>41752</v>
       </c>
@@ -12137,6 +13488,12 @@
       <c r="D126" t="s">
         <v>251</v>
       </c>
+      <c r="E126" t="s">
+        <v>879</v>
+      </c>
+      <c r="F126" t="s">
+        <v>669</v>
+      </c>
       <c r="J126" s="1">
         <v>41752</v>
       </c>
@@ -12158,6 +13515,12 @@
       <c r="D127" t="s">
         <v>253</v>
       </c>
+      <c r="E127" t="s">
+        <v>880</v>
+      </c>
+      <c r="F127" t="s">
+        <v>650</v>
+      </c>
       <c r="J127" s="1">
         <v>41752</v>
       </c>
@@ -12179,6 +13542,12 @@
       <c r="D128" t="s">
         <v>255</v>
       </c>
+      <c r="E128" t="s">
+        <v>881</v>
+      </c>
+      <c r="F128" t="s">
+        <v>650</v>
+      </c>
       <c r="J128" s="1">
         <v>41752</v>
       </c>
@@ -12200,6 +13569,9 @@
       <c r="D129" t="s">
         <v>257</v>
       </c>
+      <c r="F129" t="s">
+        <v>634</v>
+      </c>
       <c r="J129" s="1">
         <v>41752</v>
       </c>
@@ -12221,6 +13593,9 @@
       <c r="D130" t="s">
         <v>259</v>
       </c>
+      <c r="F130" t="s">
+        <v>634</v>
+      </c>
       <c r="J130" s="1">
         <v>41752</v>
       </c>
@@ -12242,6 +13617,9 @@
       <c r="D131" t="s">
         <v>261</v>
       </c>
+      <c r="F131" t="s">
+        <v>634</v>
+      </c>
       <c r="J131" s="1">
         <v>41752</v>
       </c>
@@ -12263,6 +13641,9 @@
       <c r="D132" t="s">
         <v>263</v>
       </c>
+      <c r="F132" t="s">
+        <v>634</v>
+      </c>
       <c r="J132" s="1">
         <v>41752</v>
       </c>
@@ -12284,6 +13665,12 @@
       <c r="D133" t="s">
         <v>265</v>
       </c>
+      <c r="E133" t="s">
+        <v>882</v>
+      </c>
+      <c r="F133" t="s">
+        <v>650</v>
+      </c>
       <c r="J133" s="1">
         <v>41752</v>
       </c>
@@ -12305,6 +13692,12 @@
       <c r="D134" t="s">
         <v>267</v>
       </c>
+      <c r="E134" t="s">
+        <v>883</v>
+      </c>
+      <c r="F134" t="s">
+        <v>650</v>
+      </c>
       <c r="J134" s="1">
         <v>41752</v>
       </c>
@@ -12326,6 +13719,12 @@
       <c r="D135" t="s">
         <v>269</v>
       </c>
+      <c r="E135" t="s">
+        <v>884</v>
+      </c>
+      <c r="F135" t="s">
+        <v>650</v>
+      </c>
       <c r="J135" s="1">
         <v>41752</v>
       </c>
@@ -12347,6 +13746,12 @@
       <c r="D136" t="s">
         <v>271</v>
       </c>
+      <c r="E136" t="s">
+        <v>885</v>
+      </c>
+      <c r="F136" t="s">
+        <v>650</v>
+      </c>
       <c r="J136" s="1">
         <v>41752</v>
       </c>
@@ -12368,6 +13773,12 @@
       <c r="D137" t="s">
         <v>273</v>
       </c>
+      <c r="E137" t="s">
+        <v>886</v>
+      </c>
+      <c r="F137" t="s">
+        <v>669</v>
+      </c>
       <c r="J137" s="1">
         <v>41752</v>
       </c>
@@ -12389,6 +13800,12 @@
       <c r="D138" t="s">
         <v>275</v>
       </c>
+      <c r="E138" t="s">
+        <v>887</v>
+      </c>
+      <c r="F138" t="s">
+        <v>650</v>
+      </c>
       <c r="J138" s="1">
         <v>41752</v>
       </c>
@@ -12410,6 +13827,9 @@
       <c r="D139" t="s">
         <v>277</v>
       </c>
+      <c r="F139" t="s">
+        <v>634</v>
+      </c>
       <c r="J139" s="1">
         <v>41752</v>
       </c>
@@ -12431,6 +13851,12 @@
       <c r="D140" t="s">
         <v>279</v>
       </c>
+      <c r="E140" t="s">
+        <v>888</v>
+      </c>
+      <c r="F140" t="s">
+        <v>669</v>
+      </c>
       <c r="J140" s="1">
         <v>41752</v>
       </c>
@@ -12452,6 +13878,12 @@
       <c r="D141" t="s">
         <v>281</v>
       </c>
+      <c r="E141" t="s">
+        <v>889</v>
+      </c>
+      <c r="F141" t="s">
+        <v>650</v>
+      </c>
       <c r="J141" s="1">
         <v>41752</v>
       </c>
@@ -12473,6 +13905,12 @@
       <c r="D142" t="s">
         <v>283</v>
       </c>
+      <c r="E142" t="s">
+        <v>890</v>
+      </c>
+      <c r="F142" t="s">
+        <v>650</v>
+      </c>
       <c r="J142" s="1">
         <v>41752</v>
       </c>
@@ -12491,6 +13929,12 @@
       <c r="D143" t="s">
         <v>285</v>
       </c>
+      <c r="E143" t="s">
+        <v>891</v>
+      </c>
+      <c r="F143" t="s">
+        <v>650</v>
+      </c>
       <c r="J143" s="1">
         <v>41752</v>
       </c>
@@ -12509,6 +13953,12 @@
       <c r="D144" t="s">
         <v>287</v>
       </c>
+      <c r="E144" t="s">
+        <v>892</v>
+      </c>
+      <c r="F144" t="s">
+        <v>650</v>
+      </c>
       <c r="J144" s="1">
         <v>41752</v>
       </c>
@@ -12527,6 +13977,12 @@
       <c r="D145" t="s">
         <v>289</v>
       </c>
+      <c r="E145" t="s">
+        <v>893</v>
+      </c>
+      <c r="F145" t="s">
+        <v>650</v>
+      </c>
       <c r="J145" s="1">
         <v>41752</v>
       </c>
@@ -12545,6 +14001,9 @@
       <c r="D146" t="s">
         <v>291</v>
       </c>
+      <c r="F146" t="s">
+        <v>674</v>
+      </c>
       <c r="J146" s="1">
         <v>41752</v>
       </c>
@@ -12563,6 +14022,15 @@
       <c r="D147" t="s">
         <v>293</v>
       </c>
+      <c r="E147" t="s">
+        <v>894</v>
+      </c>
+      <c r="F147" t="s">
+        <v>650</v>
+      </c>
+      <c r="H147" t="s">
+        <v>895</v>
+      </c>
       <c r="J147" s="1">
         <v>41752</v>
       </c>
@@ -12581,6 +14049,9 @@
       <c r="D148" t="s">
         <v>295</v>
       </c>
+      <c r="F148" t="s">
+        <v>634</v>
+      </c>
       <c r="J148" s="1">
         <v>41752</v>
       </c>
@@ -12599,6 +14070,12 @@
       <c r="D149" t="s">
         <v>297</v>
       </c>
+      <c r="E149" t="s">
+        <v>896</v>
+      </c>
+      <c r="F149" t="s">
+        <v>650</v>
+      </c>
       <c r="J149" s="1">
         <v>41752</v>
       </c>
@@ -12617,6 +14094,9 @@
       <c r="D150" t="s">
         <v>299</v>
       </c>
+      <c r="F150" t="s">
+        <v>674</v>
+      </c>
       <c r="J150" s="1">
         <v>41752</v>
       </c>
@@ -12635,6 +14115,12 @@
       <c r="D151" t="s">
         <v>301</v>
       </c>
+      <c r="E151" t="s">
+        <v>897</v>
+      </c>
+      <c r="F151" t="s">
+        <v>650</v>
+      </c>
       <c r="J151" s="1">
         <v>41752</v>
       </c>
@@ -12653,6 +14139,12 @@
       <c r="D152" t="s">
         <v>303</v>
       </c>
+      <c r="E152" t="s">
+        <v>898</v>
+      </c>
+      <c r="F152" t="s">
+        <v>650</v>
+      </c>
       <c r="J152" s="1">
         <v>41752</v>
       </c>
@@ -12671,6 +14163,9 @@
       <c r="D153" t="s">
         <v>305</v>
       </c>
+      <c r="F153" t="s">
+        <v>674</v>
+      </c>
       <c r="J153" s="1">
         <v>41752</v>
       </c>
@@ -12689,6 +14184,12 @@
       <c r="D154" t="s">
         <v>307</v>
       </c>
+      <c r="E154" t="s">
+        <v>899</v>
+      </c>
+      <c r="F154" t="s">
+        <v>650</v>
+      </c>
       <c r="J154" s="1">
         <v>41752</v>
       </c>
@@ -12707,6 +14208,12 @@
       <c r="D155" t="s">
         <v>309</v>
       </c>
+      <c r="E155" t="s">
+        <v>900</v>
+      </c>
+      <c r="F155" t="s">
+        <v>669</v>
+      </c>
       <c r="J155" s="1">
         <v>41752</v>
       </c>
@@ -12725,6 +14232,12 @@
       <c r="D156" t="s">
         <v>311</v>
       </c>
+      <c r="E156" t="s">
+        <v>901</v>
+      </c>
+      <c r="F156" t="s">
+        <v>650</v>
+      </c>
       <c r="J156" s="1">
         <v>41752</v>
       </c>
@@ -12743,6 +14256,12 @@
       <c r="D157" t="s">
         <v>313</v>
       </c>
+      <c r="E157" t="s">
+        <v>902</v>
+      </c>
+      <c r="F157" t="s">
+        <v>650</v>
+      </c>
       <c r="J157" s="1">
         <v>41752</v>
       </c>
@@ -12761,6 +14280,12 @@
       <c r="D158" t="s">
         <v>315</v>
       </c>
+      <c r="E158" t="s">
+        <v>906</v>
+      </c>
+      <c r="F158" t="s">
+        <v>650</v>
+      </c>
       <c r="J158" s="1">
         <v>41752</v>
       </c>
@@ -12779,6 +14304,12 @@
       <c r="D159" t="s">
         <v>317</v>
       </c>
+      <c r="E159" t="s">
+        <v>903</v>
+      </c>
+      <c r="F159" t="s">
+        <v>650</v>
+      </c>
       <c r="J159" s="1">
         <v>41752</v>
       </c>
@@ -12797,6 +14328,12 @@
       <c r="D160" t="s">
         <v>319</v>
       </c>
+      <c r="E160" t="s">
+        <v>904</v>
+      </c>
+      <c r="F160" t="s">
+        <v>650</v>
+      </c>
       <c r="J160" s="1">
         <v>41752</v>
       </c>
@@ -12814,6 +14351,15 @@
       </c>
       <c r="D161" t="s">
         <v>321</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>900</v>
+      </c>
+      <c r="F161" t="s">
+        <v>669</v>
+      </c>
+      <c r="H161" t="s">
+        <v>905</v>
       </c>
       <c r="J161" s="1">
         <v>41752</v>

</xml_diff>